<commit_message>
Diff is now using absolute values
</commit_message>
<xml_diff>
--- a/Excell Sheets/OwlExcell.xlsx
+++ b/Excell Sheets/OwlExcell.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <r>
       <t>(((</t>
@@ -422,6 +422,9 @@
   <si>
     <t>diff</t>
   </si>
+  <si>
+    <t>Constants</t>
+  </si>
 </sst>
 </file>
 
@@ -539,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
@@ -549,6 +552,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +590,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1311,7 +1316,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2232,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K16"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,45 +2249,52 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>1520</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>1540</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>10.23</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <f>POWER($C$5,2)/4</f>
         <v>1122.25</v>
       </c>
@@ -2355,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="e">
-        <f xml:space="preserve"> I9-J9</f>
+        <f>ABS(I9 - J9)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2394,8 +2405,8 @@
         <v>989.60199999999998</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K16" si="5" xml:space="preserve"> I10-J10</f>
-        <v>-12.331815878385328</v>
+        <f t="shared" ref="K10:K11" si="5">ABS(I10 - J10)</f>
+        <v>12.331815878385328</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -2434,157 +2445,10 @@
         <v>2801.0267767915625</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>2.5932555845859051</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>-2.6273773685936144</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>1709.9578202876803</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>2923955.7471629949</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="4"/>
-        <v>-56350.066803509661</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="6"/>
-        <v>1726.6812282429275</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
-        <v>1726.6812282429275</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>2.5932555845859051</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>-2.6273773685936144</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>1709.9578202876803</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
-        <v>2923955.7471629949</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="4"/>
-        <v>-56350.066803509661</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="6"/>
-        <v>1726.6812282429275</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
-        <v>1726.6812282429275</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>2.5932555845859051</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>-2.6273773685936144</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>1709.9578202876803</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="3"/>
-        <v>2923955.7471629949</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="4"/>
-        <v>-56350.066803509661</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="6"/>
-        <v>1726.6812282429275</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
-        <v>1726.6812282429275</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>2.5932555845859051</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>-2.6273773685936144</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>1709.9578202876803</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="3"/>
-        <v>2923955.7471629949</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>-56350.066803509661</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="6"/>
-        <v>1726.6812282429275</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
-        <v>1726.6812282429275</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>2.5932555845859051</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>-2.6273773685936144</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>1709.9578202876803</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
-        <v>2923955.7471629949</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>-56350.066803509661</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="6"/>
-        <v>1726.6812282429275</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
-        <v>1726.6812282429275</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Gathered data, and plotted on graph
</commit_message>
<xml_diff>
--- a/Excell Sheets/OwlExcell.xlsx
+++ b/Excell Sheets/OwlExcell.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Medarvill\Documents\GitHub\OwlProject\Excell Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medarvill\Documents\GitHub\OwlProject\Excell Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <r>
       <t>(((</t>
@@ -420,10 +420,13 @@
     <t>Reported distance</t>
   </si>
   <si>
-    <t>diff</t>
+    <t>Constants</t>
   </si>
   <si>
-    <t>Constants</t>
+    <t>Actual distance</t>
+  </si>
+  <si>
+    <t>in mm</t>
   </si>
 </sst>
 </file>
@@ -542,21 +545,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -576,6 +586,1104 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Owl</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> distance calculations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$9:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>295.81799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>506.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>779.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$9:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$15:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>297.976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>499.97899999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>765.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$15:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$21:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>253.989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>506.90100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>779.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1239.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$21:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Test 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$27:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>266.98599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>539.56100000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>738.80100000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$27:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Test 5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$33:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>258.73500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>779.14099999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1027.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1276.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1560.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$33:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$J$9:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>295.81799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>506.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>779.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1002.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>297.976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>499.97899999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>765.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1002.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>253.989</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>506.90100000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>779.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1002.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1239.06</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>266.98599999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>539.56100000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>738.80100000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1002.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1316.48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1504.79</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>258.73500000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>504.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>779.14099999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1027.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1276.98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1560.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Dist'!$K$9:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-2CA6-49CB-874A-43872CAC51C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="512615488"/>
+        <c:axId val="512615816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="512615488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reported Distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="512615816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="250"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="512615816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Actual</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="512615488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="250"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1422,7 +2530,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1942,6 +3606,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>212911</xdr:colOff>
       <xdr:row>10</xdr:row>
@@ -2236,10 +3937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,55 +3950,62 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="9"/>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1520</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1540</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6">
-        <v>10.23</v>
+      <c r="C4" s="5">
+        <v>10.98</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>POWER($C$5,2)/4</f>
         <v>1122.25</v>
       </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="12"/>
+      <c r="J7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -2321,14 +4029,14 @@
       <c r="H8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>37</v>
+      <c r="K8" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -2336,120 +4044,1148 @@
         <v>1520</v>
       </c>
       <c r="C9">
-        <v>1540</v>
+        <v>1681</v>
       </c>
       <c r="D9">
-        <f>(($C$2 - B9) * PI()) / ($C$4 * 180)</f>
+        <f t="shared" ref="D9:D10" si="0">(($C$2 - B9) * PI()) / ($C$4 * 180)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>((C9-$C$3) * PI()) / ($C$4 * 180)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" t="e">
-        <f>( $C$5 * COS(E9)) / SIN(D9 + E9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" t="e">
-        <f>POWER(F9,2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" t="e">
-        <f>F9 * $C$5 * SIN(E9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
+        <f t="shared" ref="E9:E10" si="1">((C9-$C$3) * PI()) / ($C$4 * 180)</f>
+        <v>0.22412698044735924</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F10" si="2">( $C$5 * COS(E9)) / SIN(D9 + E9)</f>
+        <v>293.91533607067043</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G10" si="3">POWER(F9,2)</f>
+        <v>86386.224777535142</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H10" si="4">F9 * $C$5 * SIN(E9)</f>
+        <v>4376.7234294011423</v>
+      </c>
+      <c r="I9">
         <f>SQRT((G9 + $C$6) - H9)</f>
-        <v>#DIV/0!</v>
+        <v>288.32577295159376</v>
       </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="e">
-        <f>ABS(I9 - J9)</f>
-        <v>#DIV/0!</v>
+        <v>295.81799999999998</v>
+      </c>
+      <c r="K9">
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>1527</v>
+        <v>1499</v>
       </c>
       <c r="C10">
-        <v>1587</v>
+        <v>1602</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:D16" si="0">(($C$2 - B10) * PI()) / ($C$4 * 180)</f>
-        <v>-1.1942624402698247E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.3380614109181167E-2</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:E16" si="1">((C10-$C$3) * PI()) / ($C$4 * 180)</f>
-        <v>8.0186192418116808E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.8552289274725341E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="2">( $C$5 * COS(E10)) / SIN(D10 + E10)</f>
-        <v>979.3828852395286</v>
+        <f t="shared" si="2"/>
+        <v>506.83879166509092</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G16" si="3">POWER(F10,2)</f>
-        <v>959190.83590010367</v>
+        <f t="shared" si="3"/>
+        <v>256885.56073652944</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H16" si="4">F10 * $C$5 * SIN(E10)</f>
-        <v>5256.0731270089345</v>
+        <f t="shared" si="4"/>
+        <v>3341.2434524247233</v>
       </c>
       <c r="I10">
-        <f>SQRT((G10 + $C$6) - H10)</f>
-        <v>977.27018412161465</v>
+        <f t="shared" ref="I10" si="5">SQRT((G10 + $C$6) - H10)</f>
+        <v>504.64499133956014</v>
       </c>
       <c r="J10">
-        <v>989.60199999999998</v>
+        <v>506.82799999999997</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K11" si="5">ABS(I10 - J10)</f>
-        <v>12.331815878385328</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>1533</v>
+        <v>1519</v>
       </c>
       <c r="C11">
+        <v>1593</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D38" si="6">(($C$2 - B11) * PI()) / ($C$4 * 180)</f>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E38" si="7">((C11-$C$3) * PI()) / ($C$4 * 180)</f>
+        <v>8.4246311799361984E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F38" si="8">( $C$5 * COS(E11)) / SIN(D11 + E11)</f>
+        <v>778.74707597350925</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G38" si="9">POWER(F11,2)</f>
+        <v>606447.00833729061</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H38" si="10">F11 * $C$5 * SIN(E11)</f>
+        <v>4390.4423334636931</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I38" si="11">SQRT((G11 + $C$6) - H11)</f>
+        <v>776.64587554678155</v>
+      </c>
+      <c r="J11">
+        <v>779.41399999999999</v>
+      </c>
+      <c r="K11">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1520</v>
+      </c>
+      <c r="C12">
+        <v>1582</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="7"/>
+        <v>6.6761228218362334E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="8"/>
+        <v>1002.0850597445962</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="9"/>
+        <v>1004174.4669633309</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="10"/>
+        <v>4478.9998403591808</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="11"/>
+        <v>1000.4087750129802</v>
+      </c>
+      <c r="J12">
+        <v>1002.64</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1520</v>
+      </c>
+      <c r="C13">
+        <v>1572</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="7"/>
+        <v>5.0865697690180824E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="8"/>
+        <v>1316.0579645671157</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="9"/>
+        <v>1732008.5661005396</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="10"/>
+        <v>4483.1940140424194</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="11"/>
+        <v>1314.7804463432278</v>
+      </c>
+      <c r="J13">
+        <v>1316.48</v>
+      </c>
+      <c r="K13">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1519</v>
+      </c>
+      <c r="C14">
         <v>1567</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-2.2179159605011031E-2</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>4.6064408410407522E-2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>2802.3694781099175</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
-        <v>7853274.6918420512</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>8645.937538722972</v>
-      </c>
-      <c r="I11">
-        <f t="shared" ref="I11:I16" si="6">SQRT((G11 + $C$6) - H11)</f>
-        <v>2801.0267767915625</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="5"/>
-        <v>2801.0267767915625</v>
+      <c r="D14">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="7"/>
+        <v>4.2917932426090065E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="8"/>
+        <v>1504.4752232693922</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="9"/>
+        <v>2263445.6974314875</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="10"/>
+        <v>4324.7927599967898</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="11"/>
+        <v>1503.4105077028996</v>
+      </c>
+      <c r="J14">
+        <v>1504.79</v>
+      </c>
+      <c r="K14">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1520</v>
+      </c>
+      <c r="C15">
+        <v>1680</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>0.22253742739454108</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="8"/>
+        <v>296.08646219946064</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="9"/>
+        <v>87667.193097792639</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="10"/>
+        <v>4378.3038026876611</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="11"/>
+        <v>290.53595181165616</v>
+      </c>
+      <c r="J15">
+        <v>297.976</v>
+      </c>
+      <c r="K15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1519</v>
+      </c>
+      <c r="C16">
+        <v>1623</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>0.13193290338390651</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="8"/>
+        <v>498.90856990398493</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="9"/>
+        <v>248909.76112363942</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="10"/>
+        <v>4397.3217649928001</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="11"/>
+        <v>495.61546521335129</v>
+      </c>
+      <c r="J16">
+        <v>499.97899999999998</v>
+      </c>
+      <c r="K16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1518</v>
+      </c>
+      <c r="C17">
+        <v>1593</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>3.1791061056363015E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>8.4246311799361984E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="8"/>
+        <v>764.62315221858478</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="9"/>
+        <v>584648.56490868505</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="10"/>
+        <v>4310.8140758670725</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="11"/>
+        <v>762.53524563315625</v>
+      </c>
+      <c r="J17">
+        <v>765.25</v>
+      </c>
+      <c r="K17">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1520</v>
+      </c>
+      <c r="C18">
+        <v>1582</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>6.6761228218362334E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="8"/>
+        <v>1002.0850597445962</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="9"/>
+        <v>1004174.4669633309</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="10"/>
+        <v>4478.9998403591808</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="11"/>
+        <v>1000.4087750129802</v>
+      </c>
+      <c r="J18">
+        <v>1002.64</v>
+      </c>
+      <c r="K18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1520</v>
+      </c>
+      <c r="C19">
+        <v>1572</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="7"/>
+        <v>5.0865697690180824E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="8"/>
+        <v>1316.0579645671157</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="9"/>
+        <v>1732008.5661005396</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="10"/>
+        <v>4483.1940140424194</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="11"/>
+        <v>1314.7804463432278</v>
+      </c>
+      <c r="J19">
+        <v>1316.48</v>
+      </c>
+      <c r="K19">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1519</v>
+      </c>
+      <c r="C20">
+        <v>1567</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>4.2917932426090065E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="8"/>
+        <v>1504.4752232693922</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="9"/>
+        <v>2263445.6974314875</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="10"/>
+        <v>4324.7927599967898</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="11"/>
+        <v>1503.4105077028996</v>
+      </c>
+      <c r="J20">
+        <v>1504.79</v>
+      </c>
+      <c r="K20">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1439</v>
+      </c>
+      <c r="C21">
+        <v>1624</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="6"/>
+        <v>0.12875379727827019</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="7"/>
+        <v>0.13352245643672467</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>256.10820191838519</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="9"/>
+        <v>65591.411089868358</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="10"/>
+        <v>2284.3433636581876</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="11"/>
+        <v>253.82930824908729</v>
+      </c>
+      <c r="J21">
+        <v>253.989</v>
+      </c>
+      <c r="K21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1496</v>
+      </c>
+      <c r="C22">
+        <v>1599</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="6"/>
+        <v>3.8149273267635612E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>9.3783630116270889E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="8"/>
+        <v>507.07199726659775</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="9"/>
+        <v>257122.01041193653</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="10"/>
+        <v>3181.5199625896239</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="11"/>
+        <v>505.03736539918202</v>
+      </c>
+      <c r="J22">
+        <v>506.90100000000001</v>
+      </c>
+      <c r="K22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1519</v>
+      </c>
+      <c r="C23">
+        <v>1593</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>8.4246311799361984E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="8"/>
+        <v>778.74707597350925</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="9"/>
+        <v>606447.00833729061</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="10"/>
+        <v>4390.4423334636931</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="11"/>
+        <v>776.64587554678155</v>
+      </c>
+      <c r="J23">
+        <v>779.41399999999999</v>
+      </c>
+      <c r="K23">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1519</v>
+      </c>
+      <c r="C24">
+        <v>1581</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>6.5171675165544174E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="8"/>
+        <v>1002.1902937809612</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="9"/>
+        <v>1004385.3849487692</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="10"/>
+        <v>4372.9690378278756</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="11"/>
+        <v>1000.5671721133675</v>
+      </c>
+      <c r="J24">
+        <v>1002.7</v>
+      </c>
+      <c r="K24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1518</v>
+      </c>
+      <c r="C25">
+        <v>1572</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="6"/>
+        <v>3.1791061056363015E-3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="7"/>
+        <v>5.0865697690180824E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="8"/>
+        <v>1238.7116570976473</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="9"/>
+        <v>1534406.5694295992</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="10"/>
+        <v>4219.7113164779075</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="11"/>
+        <v>1237.460750130331</v>
+      </c>
+      <c r="J25">
+        <v>1239.06</v>
+      </c>
+      <c r="K25">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1519</v>
+      </c>
+      <c r="C26">
+        <v>1567</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>4.2917932426090065E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="8"/>
+        <v>1504.4752232693922</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="9"/>
+        <v>2263445.6974314875</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="10"/>
+        <v>4324.7927599967898</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="11"/>
+        <v>1503.4105077028996</v>
+      </c>
+      <c r="J26">
+        <v>1504.79</v>
+      </c>
+      <c r="K26">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1425</v>
+      </c>
+      <c r="C27">
+        <v>1602</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="6"/>
+        <v>0.15100754001772432</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="7"/>
+        <v>9.8552289274725341E-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="8"/>
+        <v>269.96348507075345</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="9"/>
+        <v>72880.283271546927</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="10"/>
+        <v>1779.685654926049</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="11"/>
+        <v>268.74308850018986</v>
+      </c>
+      <c r="J27">
+        <v>266.98599999999999</v>
+      </c>
+      <c r="K27">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1495</v>
+      </c>
+      <c r="C28">
+        <v>1593</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="6"/>
+        <v>3.9738826320453766E-2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>8.4246311799361984E-2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="8"/>
+        <v>539.85286707233831</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="9"/>
+        <v>291441.11808622378</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="10"/>
+        <v>3043.5977926121541</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="11"/>
+        <v>538.07041388057348</v>
+      </c>
+      <c r="J28">
+        <v>539.56100000000004</v>
+      </c>
+      <c r="K28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1505</v>
+      </c>
+      <c r="C29">
+        <v>1582</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="6"/>
+        <v>2.3843295792272259E-2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="7"/>
+        <v>6.6761228218362334E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="8"/>
+        <v>738.84055188929483</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="9"/>
+        <v>545885.36111607775</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="10"/>
+        <v>3302.3810521698447</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="11"/>
+        <v>737.36370270302018</v>
+      </c>
+      <c r="J29">
+        <v>738.80100000000004</v>
+      </c>
+      <c r="K29">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1519</v>
+      </c>
+      <c r="C30">
+        <v>1581</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="7"/>
+        <v>6.5171675165544174E-2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="8"/>
+        <v>1002.1902937809612</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="9"/>
+        <v>1004385.3849487692</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="10"/>
+        <v>4372.9690378278756</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="11"/>
+        <v>1000.5671721133675</v>
+      </c>
+      <c r="J30">
+        <v>1002.7</v>
+      </c>
+      <c r="K30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1520</v>
+      </c>
+      <c r="C31">
+        <v>1572</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="7"/>
+        <v>5.0865697690180824E-2</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="8"/>
+        <v>1316.0579645671157</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="9"/>
+        <v>1732008.5661005396</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="10"/>
+        <v>4483.1940140424194</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="11"/>
+        <v>1314.7804463432278</v>
+      </c>
+      <c r="J31">
+        <v>1316.48</v>
+      </c>
+      <c r="K31">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1519</v>
+      </c>
+      <c r="C32">
+        <v>1567</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="7"/>
+        <v>4.2917932426090065E-2</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="8"/>
+        <v>1504.4752232693922</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>2263445.6974314875</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>4324.7927599967898</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="11"/>
+        <v>1503.4105077028996</v>
+      </c>
+      <c r="J32">
+        <v>1504.79</v>
+      </c>
+      <c r="K32">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1445</v>
+      </c>
+      <c r="C33">
+        <v>1627</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="6"/>
+        <v>0.1192164789613613</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="7"/>
+        <v>0.13829111559517909</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="8"/>
+        <v>260.57274114055519</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>67898.15342550278</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>2406.6498506695316</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="11"/>
+        <v>258.09640364567895</v>
+      </c>
+      <c r="J33">
+        <v>258.73500000000001</v>
+      </c>
+      <c r="K33">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1499</v>
+      </c>
+      <c r="C34">
+        <v>1602</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="6"/>
+        <v>3.3380614109181167E-2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="7"/>
+        <v>9.8552289274725341E-2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>506.83879166509092</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>256885.56073652944</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="10"/>
+        <v>3341.2434524247233</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>504.64499133956014</v>
+      </c>
+      <c r="J34">
+        <v>504.82799999999997</v>
+      </c>
+      <c r="K34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1519</v>
+      </c>
+      <c r="C35">
+        <v>1593</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="7"/>
+        <v>8.4246311799361984E-2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>778.74707597350925</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>606447.00833729061</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="10"/>
+        <v>4390.4423334636931</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="11"/>
+        <v>776.64587554678155</v>
+      </c>
+      <c r="J35">
+        <v>779.14099999999996</v>
+      </c>
+      <c r="K35">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1519</v>
+      </c>
+      <c r="C36">
+        <v>1580</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="7"/>
+        <v>6.3582122112726028E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="8"/>
+        <v>1026.7032694506295</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>1054119.6035006118</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="10"/>
+        <v>4370.8118079544438</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="11"/>
+        <v>1025.1200133119328</v>
+      </c>
+      <c r="J36">
+        <v>1027.2</v>
+      </c>
+      <c r="K36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1505</v>
+      </c>
+      <c r="C37">
+        <v>1558</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="6"/>
+        <v>2.3843295792272259E-2</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="7"/>
+        <v>2.8611954950726711E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="8"/>
+        <v>1277.3421023475823</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>1631602.8464297415</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="10"/>
+        <v>2448.3319802240621</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="11"/>
+        <v>1276.8229182034279</v>
+      </c>
+      <c r="J37">
+        <v>1276.98</v>
+      </c>
+      <c r="K37">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1510</v>
+      </c>
+      <c r="C38">
+        <v>1557</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="6"/>
+        <v>1.5895530528181507E-2</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="7"/>
+        <v>2.7022401897908561E-2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="8"/>
+        <v>1561.0282462179287</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>2436809.1854902222</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="10"/>
+        <v>2825.8991410678427</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="11"/>
+        <v>1560.4824690938231</v>
+      </c>
+      <c r="J38">
+        <v>1560.86</v>
+      </c>
+      <c r="K38">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Owl Excell sheet
</commit_message>
<xml_diff>
--- a/Excell Sheets/OwlExcell.xlsx
+++ b/Excell Sheets/OwlExcell.xlsx
@@ -1147,7 +1147,43 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.28496576357707354"/>
+                  <c:y val="0.50099807368868243"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3939,7 +3975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>

</xml_diff>